<commit_message>
corrected MODEL_EXEC_2: model must be csvread.acs
</commit_message>
<xml_diff>
--- a/Tests/integrationTests/04_Model execution/Test_cases_Model_Execution.xlsx
+++ b/Tests/integrationTests/04_Model execution/Test_cases_Model_Execution.xlsx
@@ -265,12 +265,6 @@
 4. Click on button 'Read File' and select created file of test MODEL_EXEC_1</t>
   </si>
   <si>
-    <t>ARE start file: Are.exe (start.sh - Linux)
-ACS: ACS.exe
-model: ReadWriteCSV\csvwriter.acs
-Test MODEL_EXEC_1</t>
-  </si>
-  <si>
     <t>1. The model must be deployed and started successfully.
 2. After clicking 'Read file' the Oscilloscope must show a correct sinus signal</t>
   </si>
@@ -465,6 +459,12 @@
   </si>
   <si>
     <t>Environment (OS + Version, Architecture, Java Version):</t>
+  </si>
+  <si>
+    <t>ARE start file: Are.exe (start.sh - Linux)
+ACS: ACS.exe
+model: ReadWriteCSV\csvread.acs
+Test MODEL_EXEC_1</t>
   </si>
 </sst>
 </file>
@@ -846,7 +846,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -857,7 +857,7 @@
   <dimension ref="A1:F85"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,10 +874,10 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>89</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.4">
@@ -888,7 +888,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.4">
@@ -899,7 +899,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
@@ -951,13 +951,13 @@
         <v>28</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>46</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F8" s="5"/>
     </row>
@@ -969,13 +969,13 @@
         <v>29</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="F9" s="5"/>
     </row>
@@ -987,13 +987,13 @@
         <v>30</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="F10" s="5"/>
     </row>
@@ -1005,13 +1005,13 @@
         <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="F11" s="5"/>
     </row>
@@ -1023,13 +1023,13 @@
         <v>32</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="5"/>
     </row>
@@ -1041,13 +1041,13 @@
         <v>33</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F13" s="5"/>
     </row>
@@ -1059,13 +1059,13 @@
         <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" s="5"/>
     </row>
@@ -1077,13 +1077,13 @@
         <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F15" s="5"/>
     </row>
@@ -1095,13 +1095,13 @@
         <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="F16" s="5"/>
     </row>
@@ -1113,13 +1113,13 @@
         <v>37</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="F17" s="5"/>
     </row>
@@ -1128,16 +1128,16 @@
         <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F18" s="5"/>
     </row>
@@ -1146,7 +1146,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1158,7 +1158,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1173,13 +1173,13 @@
         <v>38</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="F21" s="5"/>
     </row>
@@ -1191,13 +1191,13 @@
         <v>40</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="5"/>
     </row>
@@ -1209,31 +1209,31 @@
         <v>41</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="F23" s="5"/>
     </row>
     <row r="24" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="C24" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="F24" s="5"/>
     </row>

</xml_diff>